<commit_message>
Se actualzian imagenes del dashboard
</commit_message>
<xml_diff>
--- a/Dashboard_Flota.xlsx
+++ b/Dashboard_Flota.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mini_proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB574AD2-C94F-4725-BC7D-007569551FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7362DA6-EC07-4CA7-B235-11143AD8D996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MovimientosFlota" sheetId="1" r:id="rId1"/>
@@ -226,7 +226,7 @@
     <tableColumn id="7" xr3:uid="{AD7543F6-F984-449C-947B-CDBA92192D89}" name="Tiempo_Min"/>
     <tableColumn id="8" xr3:uid="{DC09DE5F-D606-4E33-A6CC-2A3731A39CA0}" name="Estado"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -238,7 +238,7 @@
     <tableColumn id="2" xr3:uid="{991C354C-C6B4-4124-A350-ED9C6AE922AA}" name="Nombre"/>
     <tableColumn id="3" xr3:uid="{7136D32D-6CF2-4F25-B579-57B786DD2CEF}" name="Documento"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -250,7 +250,7 @@
     <tableColumn id="2" xr3:uid="{2CE61E9C-C822-401E-AFBA-164B6DA1F683}" name="Placa"/>
     <tableColumn id="3" xr3:uid="{0BA651A5-EF1D-4B9E-B69E-89E51DD9FF83}" name="Tipo"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -541,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,7 +854,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>